<commit_message>
changed q3, and last table; added expected res for each step
</commit_message>
<xml_diff>
--- a/lab5/LAB5_PRIKHODKO_YURIY.xlsx
+++ b/lab5/LAB5_PRIKHODKO_YURIY.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Номер Тестового випадку</t>
   </si>
@@ -40,7 +40,7 @@
     <t>Підготовка: Підготувати системний лічильник здатний зафіксувати точний час між настисканням кнопки миші, та відгуком програми. Кроки: 1. Запустіть програму 2. Виміряйте час від початку запуску, до повного завантаження, виміряйте завантаження процесора за допомогою панелі задач. 3. Натисніть на кнопку закриття програми 4. Виміряйте час від натискання кнопки закриття до повного припинення процесу програми, виміряйте завантаження процесора за допомогою панелі задач.</t>
   </si>
   <si>
-    <t>Час запуску та закриття програми не перевищує 2 с; використання ресурсів процесора не перевищує 20%.</t>
+    <t>1. Програма запустилась успішно 2. Час запуску програми не перевищує 2 с; використання ресурсів процесора не перевищує 20%. 3. Програма закрилась успішно 4. Час закриття програми не перевищує 2 с; використання ресурсів процесора не перевищує 20%.</t>
   </si>
   <si>
     <t>TC-002</t>
@@ -55,7 +55,7 @@
     <t>Підготовка: Підготувати системний лічильник здатний зафіксувати точний час між настисканням кнопки миші, та відгуком програми. Кроки: 1. Відкрийте програму 2. Натисніть на кнопку пункту меню 3. Виміряйте час від натискання до відкриття пункту меню.</t>
   </si>
   <si>
-    <t>Час реакції на вибір пункта меню не перевищує 2 с.</t>
+    <t>1. Програма відкрилась без помилок 2. Відкрився обраний пункт меню 3. Час реакції на вибір пункта меню не перевищує 2 с.</t>
   </si>
   <si>
     <t>TC-003</t>
@@ -70,7 +70,10 @@
     <t>Підготовка: Підготувати системний лічильник здатний зафіксувати точний час між настисканням кнопки миші, та відгуком програми. Кроки: 1. Запустіть програму 2. Натисніть ліву кнопку миші на клітинці ігрового поля. 3. Виміряйте час від натискання до реакції програми. 4. Натисніть праву кнопку миші на клітинці ігрового поля. 5. Виміряйте час між натисканням кнопки миші та реакцією програми</t>
   </si>
   <si>
-    <t>Час реакції на натискання кнопок миші не перевищує 0.2 с.</t>
+    <t>1. Програма запустилась без помилок 2. Клітинка на яку натиснули відкрилась 3. Час реакції на натискання кнопок миші не перевищує 0.2 с. 4. Клітинка на яку натиснули позначилась прапором. 5.Час реакції на натискання кнопок миші не перевищує 0.2 с. 4.</t>
+  </si>
+  <si>
+    <t>TC-004</t>
   </si>
   <si>
     <t>P-40</t>
@@ -82,7 +85,7 @@
     <t>Підготовка: Підготувати системний лічильник здатний зафіксувати точний час між настисканням кнопки миші, та відгуком програми. Кроки: 1. Відкрийте програму 2. Натисніть кнопку старту нової гри. 3. Виміряйте час до оновлення ігрового поля.</t>
   </si>
   <si>
-    <t>Час між натисканням кнопки старту нової гри та оновленням ігрового поля не перевищує 1 с.</t>
+    <t>1. Програма запустилась успішно 2. Почалась нова гра, ігрове поле оновилось 3. Час між натисканням кнопки старту нової гри та оновленням ігрового поля не перевищує 1 с.</t>
   </si>
 </sst>
 </file>
@@ -444,19 +447,19 @@
     </row>
     <row r="5" ht="126.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>